<commit_message>
anchor size constraint up down timer
</commit_message>
<xml_diff>
--- a/решения/Flip/wheel.xlsx
+++ b/решения/Flip/wheel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reynikovanton/Desktop/APP/development/Locity/решения/Flip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3787314D-A2D8-D846-8E72-F29E35C7F05A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1202EAD8-26A7-B243-AA46-06ED81E960E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="1720" windowWidth="25820" windowHeight="20300" xr2:uid="{2D5C6F0C-BF6E-1B43-B662-86FAADCFD52C}"/>
+    <workbookView xWindow="10660" yWindow="2960" windowWidth="25820" windowHeight="20300" xr2:uid="{2D5C6F0C-BF6E-1B43-B662-86FAADCFD52C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -307,19 +307,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.0000000000000009</c:v>
+                  <c:v>10.416666666666668</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>28.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>14.583333333333334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1496,7 +1496,7 @@
   <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202"/>
+      <selection activeCell="A97" sqref="A2:A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1518,21 +1518,21 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
         <f t="array" ref="D2:D7">FREQUENCY(A2:A201,C2:C6)</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="6">
         <f>D2/D8*100</f>
-        <v>7.0000000000000009</v>
+        <v>10.416666666666668</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -1543,20 +1543,20 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="6">
         <f>D3/D8*100</f>
-        <v>20</v>
+        <v>28.125</v>
       </c>
       <c r="G3">
         <v>26</v>
@@ -1567,20 +1567,20 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="6">
         <f>D4/D8*100</f>
-        <v>25</v>
+        <v>14.583333333333334</v>
       </c>
       <c r="G4">
         <v>29</v>
@@ -1591,20 +1591,20 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="6">
         <f>D5/D8*100</f>
-        <v>22</v>
+        <v>21.875</v>
       </c>
       <c r="G5">
         <v>22</v>
@@ -1621,14 +1621,14 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="8">
         <f>D6/D8*100</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6">
         <v>18</v>
@@ -1660,56 +1660,56 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f>SUM(D2:D6)</f>
-        <v>200</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
@@ -1724,12 +1724,12 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
@@ -1739,7 +1739,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
@@ -1749,12 +1749,12 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
@@ -1764,27 +1764,27 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
@@ -1799,7 +1799,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
@@ -1809,12 +1809,12 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
@@ -1829,32 +1829,32 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
@@ -1864,27 +1864,27 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
@@ -1894,12 +1894,12 @@
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
@@ -1909,147 +1909,147 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
@@ -2059,7 +2059,7 @@
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
@@ -2069,7 +2069,7 @@
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
@@ -2079,7 +2079,7 @@
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
@@ -2089,548 +2089,31 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A128">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A129">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A130">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A139">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A140">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A141">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A143">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A144">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A145">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A146">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A147">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A149">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A150">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A151">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A153">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A154">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A155">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A156">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A157">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A158">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A159">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A160">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A164">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A165">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A167">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A168">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A169">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A170">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A171">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A172">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A173">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A174">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A175">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A176">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A177">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A178">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A179">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A180">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A181">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A182">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A183">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A184">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A185">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A186">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A187">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A188">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A189">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A190">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A191">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A192">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A193">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A194">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A195">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A196">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A197">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A198">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A199">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A200">
         <v>5</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A201" s="9">
-        <v>2</v>
-      </c>
+      <c r="A201" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>